<commit_message>
SamplePathology,SampleSite, SampleType, StageOfDisease were updated
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_Canine_Filter_SamplePatho-Astrocytoma.xlsx
+++ b/InputFiles/TC01_Canine_Filter_SamplePatho-Astrocytoma.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sohilz2\Commons_Automation\InputFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\podagatlapalll2\ICDC Automation\Lakshmi0412\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29F0C101-C1A3-4F53-9587-AD9CB215820D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5AF2B5F-33A6-463B-B4B4-6A3AE9674C08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-105" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="startup" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
   <si>
     <t>WebExcel</t>
   </si>
@@ -63,29 +63,95 @@
     <t>TC01_Canine_Filter_SamplePatho-Astrocytoma_WebData.xlsx</t>
   </si>
   <si>
-    <t>MATCH (s:study)
-  WITH COLLECT(DISTINCT(s.clinical_study_designation)) AS all_studies
-  MATCH (d:demographic) WITH COLLECT(DISTINCT(d.breed)) AS all_breeds, COLLECT(DISTINCT(d.sex)) AS all_sexes, all_studies
-  MATCH (d:diagnosis)
-  WITH COLLECT(DISTINCT(d.disease_term)) AS all_diseases, all_breeds, all_sexes, all_studies
-  MATCH (p:program)&lt;-[*]-(s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (c)&lt;--(diag:diagnosis)
-  MATCH (samp:sample)-[*]-&gt;(c)
-  MATCH (f:file)-[*]-&gt;(c)
-  WHERE samp.specific_sample_pathology IN ["Astrocytoma"]  
-  WITH DISTINCT c AS c, p, s, demo, diag, f, samp
-  RETURN count(DISTINCT(f)) as number_of_files ,
-             count(DISTINCT(samp)) as number_of_sample ,
-             count(DISTINCT(c.case_id)) as number_of_cases ,
-             count(DISTINCT(s.clinical_study_designation)) as number_of_study</t>
+    <t>StudyFilesTab</t>
+  </si>
+  <si>
+    <t>MATCH (f:file)--&gt;(s:study)
+MATCH (s)&lt;--(c:case)&lt;--(diag:diagnosis)
+MATCH (c)&lt;--(demo:demographic)
+MATCH (samp:sample)--&gt;(c)
+WHERE samp.specific_sample_pathology IN ['Astrocytoma']
+WITH
+        DISTINCT f, c, demo, diag, s,
+        ['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units,
+        toInteger(floor(log(f.file_size)/log(1024))) as i,
+        2 as precision
+WITH
+        f, c, demo, diag, s,
+        f.file_size /(1024^i) AS value, 10^precision AS factor,
+        units[i] as unit
+        WITH
+        f,  c, demo, diag, s, unit,
+        round(factor * value)/factor AS size
+RETURN DISTINCT
+  coalesce(f.file_name, '') AS `File Name`,
+  coalesce(f.file_type, '') AS `File Type`,
+  coalesce("study", '') AS `Association`,
+  coalesce(f.file_description, '') AS `Description`,
+  coalesce(f.file_format, '') AS  Format,
+  CASE size % 1 WHEN 0 THEN apoc.convert.toInteger(size)+' ' +unit ELSE size+' ' +unit END AS Size,
+  coalesce(s.clinical_study_designation,'') AS `Study Code`
+  order by 'File Name' asc
+  limit 100</t>
+  </si>
+  <si>
+    <t>MATCH (p:program)&lt;--(s:study)&lt;--(c)
+MATCH (cf)--&gt;(samp:sample)
+WHERE samp.specific_sample_pathology IN ['Astrocytoma']
+MATCH (cf:file)-[*]-&gt;(c:case)
+OPTIONAL MATCH (sf:file)--&gt;(s)
+RETURN
+    count(distinct p) AS Programs,
+    count(distinct s) AS Studies,
+    count(distinct c) AS Cases,
+    count(distinct samp) AS Samples,
+    count(distinct cf) AS `Case Files`,
+    count(distinct sf) AS `Study Files`</t>
+  </si>
+  <si>
+    <t>MATCH (p:program)&lt;--(s:study)&lt;--(c)
+MATCH (cf)--&gt;(samp:sample)
+WHERE samp.specific_sample_pathology IN ['Astrocytoma']
+MATCH (cf:file)-[*]-&gt;(c:case)
+OPTIONAL MATCH (sf:file)--&gt;(s)
+RETURN
+    count(distinct p) AS Programs,
+    count(distinct s) AS Studies,
+    count(distinct c) AS Cases,
+   count(distinct samp) AS Samples,
+    count(distinct cf) AS `Case Files`,
+    count(distinct sf) AS `Study Files`</t>
+  </si>
+  <si>
+    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
+MATCH (c)&lt;--(diag:diagnosis)
+OPTIONAL MATCH (co:cohort)&lt;-[*]-(c)
+MATCH (samp:sample)--&gt;(c)
+WHERE  samp.specific_sample_pathology in ['Astrocytoma']
+WITH DISTINCT c, s, demo, diag, co, demo.patient_age_at_enrollment AS age, demo.weight as weight
+RETURN  coalesce(c.case_id, '') AS `Case ID` ,
+        coalesce(s.clinical_study_designation, '') AS `Study Code` ,
+        coalesce(s.clinical_study_type, '') AS  `Study Type`,
+        coalesce(demo.breed, '') AS Breed ,
+        coalesce(diag.disease_term, '') AS Diagnosis ,
+        coalesce(diag.stage_of_disease, '') AS `Stage of Disease` ,
+  coalesce(CASE age % 1 WHEN 0 THEN apoc.convert.toInteger(age) ELSE age END, '') AS Age,
+       coalesce(demo.sex, '') AS Sex,
+       coalesce(demo.neutered_indicator, '') AS `Neutered Status`,
+coalesce(CASE weight % 1 WHEN 0 THEN apoc.convert.toInteger(weight) ELSE weight END, '') AS `Weight (kg)`,
+       coalesce(diag.best_response, '') AS `Response to Treatment`,
+       coalesce(co.cohort_description, '') AS `Cohort`
+order by c.case_id asc
+limit 100</t>
   </si>
   <si>
     <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (samp:sample)--&gt;(c)&lt;--(diag:diagnosis) 
- WHERE samp.specific_sample_pathology IN ["Astrocytoma"]  
+WHERE  samp.specific_sample_pathology IN ['Astrocytoma']
 WITH DISTINCT samp AS samp, c, demo, diag
 RETURN  coalesce(samp.sample_id, '') AS `Sample ID`, 
         coalesce(c.case_id, '') AS `Case ID`, 
-        coalesce(demo.breed,'') AS Breed , 
-        coalesce(diag.disease_term,'') AS Diagnosis , 
+        coalesce(demo.breed,'') AS Breed,
+        coalesce(diag.disease_term,'') AS Diagnosis, 
         coalesce(samp.sample_site, '') AS `Sample Site`,
         coalesce(samp.summarized_sample_type, '') AS `Sample Type`,
         coalesce(samp.specific_sample_pathology, '') AS `Pathology/Morphology`,
@@ -93,50 +159,51 @@
         coalesce(samp.sample_chronology, '') AS `Sample Chronology`,
         coalesce(samp.percentage_tumor, '') AS `Percentage Tumor`,
         coalesce(samp.necropsy_sample, '') AS `Necropsy Sample`,
-        coalesce(samp.sample_preservation, '') AS `Sample Preservation`</t>
+        coalesce(samp.sample_preservation, '') AS `Sample Preservation`
+order by samp.sample_id asc
+limit 200</t>
   </si>
   <si>
     <t>MATCH (f:file)--&gt;(parent)
 WITH DISTINCT f, parent
 MATCH (f)-[*]-&gt;(c:case)&lt;--(demo:demographic)
- MATCH (s:study)&lt;-[*]-(c)&lt;--(diag:diagnosis)
- MATCH (samp:sample)--&gt;(c) 
- WHERE samp.specific_sample_pathology IN ["Astrocytoma"]  
-WITH DISTINCT f, parent, c, demo, diag, s
-RETURN coalesce(f.file_name, '') AS `File Name`, 
+MATCH (s:study)&lt;-[*]-(c)&lt;--(diag:diagnosis)
+MATCH (f)--&gt;(samp:sample)
+WHERE samp.specific_sample_pathology IN ['Astrocytoma']
+ MATCH (f)-[*]-&gt;(samp:sample)
+WITH
+        DISTINCT f, parent, c, demo, diag, s, samp,
+        ['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units,
+        toInteger(floor(log(f.file_size)/log(1024))) as i,
+        2 as precision
+WITH
+        f, parent, c, demo, diag, s, samp,
+        f.file_size /(1024^i) AS value,
+        10^precision AS factor,
+        units[i] as unit
+WITH
+        f, parent, c, demo, diag, s, samp, unit,
+        round(factor * value)/factor AS size
+RETURN
+        coalesce(f.file_name, '') AS `File Name`,
+        coalesce(f.file_format, '') AS `Format`,
+        coalesce(f.file_type, '') AS `File Type`,
+        CASE size % 1 WHEN 0 THEN apoc.convert.toInteger(size)+' ' +unit ELSE size+' ' +unit END AS Size,
         coalesce(labels(parent)[0], '') AS `Association`,
         coalesce(f.file_description, '') AS `Description`,
-        coalesce(f.file_format, '') AS `Format`,
-        coalesce(f.file_size, '') AS `Size`,
-        coalesce(c.case_id, '') AS `Case ID`, 
-        coalesce(diag.disease_term,'') AS Diagnosis , 
-        coalesce(s.clinical_study_designation,'') AS `Study Code`</t>
-  </si>
-  <si>
-    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
-MATCH (c)&lt;--(diag:diagnosis)
-MATCH (samp:sample)--&gt;(c) 
- WHERE samp.specific_sample_pathology IN ["Astrocytoma"]  
-OPTIONAL MATCH (co:cohort)&lt;-[*]-(c)
-  WITH DISTINCT c, s, demo, diag, co
-RETURN  coalesce(c.case_id, '') AS `Case ID` ,
-        coalesce(s.clinical_study_designation, '') AS `Study Code` ,
-        coalesce(s.clinical_study_type, '') AS  `Study Type`,
-        coalesce(demo.breed, '') AS Breed ,
-        coalesce(diag.disease_term, '') AS Diagnosis ,
-        coalesce(diag.stage_of_disease, '') AS `Stage of Disease` ,
-        coalesce(demo.patient_age_at_enrollment, '') AS Age ,
-        coalesce(demo.sex, '') AS Sex ,
-        coalesce(demo.neutered_indicator, '') AS `Neutered Status`,
-        coalesce(demo.weight, '') AS `Weight (kg)`,
-        coalesce(diag.best_response, '') AS `Response to Treatment`</t>
+        coalesce(samp.sample_id, '') AS `Sample ID`,
+        coalesce(c.case_id, '') AS `Case ID`,
+        coalesce(demo.breed,'') AS Breed ,
+        coalesce(diag.disease_term,'') AS Diagnosis
+        order by f.file_name asc
+        limit 100</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -153,6 +220,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -179,9 +253,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -499,22 +579,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="87.6640625" customWidth="1"/>
-    <col min="3" max="3" width="75.77734375" customWidth="1"/>
-    <col min="4" max="4" width="70.21875" customWidth="1"/>
-    <col min="5" max="5" width="28.5546875" customWidth="1"/>
+    <col min="1" max="1" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="87.6328125" customWidth="1"/>
+    <col min="3" max="3" width="75.81640625" customWidth="1"/>
+    <col min="4" max="4" width="70.1796875" customWidth="1"/>
+    <col min="5" max="5" width="28.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -531,15 +611,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="244.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="304.5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
@@ -548,15 +628,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="244.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>10</v>
+      <c r="B3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
@@ -565,20 +645,37 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="244.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="D4" t="s">
         <v>8</v>
       </c>
       <c r="E4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Manually add ICDC TCL01 Test for Prasanna
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_Canine_Filter_SamplePatho-Astrocytoma.xlsx
+++ b/InputFiles/TC01_Canine_Filter_SamplePatho-Astrocytoma.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sohilz2\Commons_Automation\InputFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\podagatlapalll2\ICDC Automation\Lakshmi0412\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29F0C101-C1A3-4F53-9587-AD9CB215820D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5AF2B5F-33A6-463B-B4B4-6A3AE9674C08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-105" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="startup" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
   <si>
     <t>WebExcel</t>
   </si>
@@ -63,29 +63,95 @@
     <t>TC01_Canine_Filter_SamplePatho-Astrocytoma_WebData.xlsx</t>
   </si>
   <si>
-    <t>MATCH (s:study)
-  WITH COLLECT(DISTINCT(s.clinical_study_designation)) AS all_studies
-  MATCH (d:demographic) WITH COLLECT(DISTINCT(d.breed)) AS all_breeds, COLLECT(DISTINCT(d.sex)) AS all_sexes, all_studies
-  MATCH (d:diagnosis)
-  WITH COLLECT(DISTINCT(d.disease_term)) AS all_diseases, all_breeds, all_sexes, all_studies
-  MATCH (p:program)&lt;-[*]-(s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (c)&lt;--(diag:diagnosis)
-  MATCH (samp:sample)-[*]-&gt;(c)
-  MATCH (f:file)-[*]-&gt;(c)
-  WHERE samp.specific_sample_pathology IN ["Astrocytoma"]  
-  WITH DISTINCT c AS c, p, s, demo, diag, f, samp
-  RETURN count(DISTINCT(f)) as number_of_files ,
-             count(DISTINCT(samp)) as number_of_sample ,
-             count(DISTINCT(c.case_id)) as number_of_cases ,
-             count(DISTINCT(s.clinical_study_designation)) as number_of_study</t>
+    <t>StudyFilesTab</t>
+  </si>
+  <si>
+    <t>MATCH (f:file)--&gt;(s:study)
+MATCH (s)&lt;--(c:case)&lt;--(diag:diagnosis)
+MATCH (c)&lt;--(demo:demographic)
+MATCH (samp:sample)--&gt;(c)
+WHERE samp.specific_sample_pathology IN ['Astrocytoma']
+WITH
+        DISTINCT f, c, demo, diag, s,
+        ['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units,
+        toInteger(floor(log(f.file_size)/log(1024))) as i,
+        2 as precision
+WITH
+        f, c, demo, diag, s,
+        f.file_size /(1024^i) AS value, 10^precision AS factor,
+        units[i] as unit
+        WITH
+        f,  c, demo, diag, s, unit,
+        round(factor * value)/factor AS size
+RETURN DISTINCT
+  coalesce(f.file_name, '') AS `File Name`,
+  coalesce(f.file_type, '') AS `File Type`,
+  coalesce("study", '') AS `Association`,
+  coalesce(f.file_description, '') AS `Description`,
+  coalesce(f.file_format, '') AS  Format,
+  CASE size % 1 WHEN 0 THEN apoc.convert.toInteger(size)+' ' +unit ELSE size+' ' +unit END AS Size,
+  coalesce(s.clinical_study_designation,'') AS `Study Code`
+  order by 'File Name' asc
+  limit 100</t>
+  </si>
+  <si>
+    <t>MATCH (p:program)&lt;--(s:study)&lt;--(c)
+MATCH (cf)--&gt;(samp:sample)
+WHERE samp.specific_sample_pathology IN ['Astrocytoma']
+MATCH (cf:file)-[*]-&gt;(c:case)
+OPTIONAL MATCH (sf:file)--&gt;(s)
+RETURN
+    count(distinct p) AS Programs,
+    count(distinct s) AS Studies,
+    count(distinct c) AS Cases,
+    count(distinct samp) AS Samples,
+    count(distinct cf) AS `Case Files`,
+    count(distinct sf) AS `Study Files`</t>
+  </si>
+  <si>
+    <t>MATCH (p:program)&lt;--(s:study)&lt;--(c)
+MATCH (cf)--&gt;(samp:sample)
+WHERE samp.specific_sample_pathology IN ['Astrocytoma']
+MATCH (cf:file)-[*]-&gt;(c:case)
+OPTIONAL MATCH (sf:file)--&gt;(s)
+RETURN
+    count(distinct p) AS Programs,
+    count(distinct s) AS Studies,
+    count(distinct c) AS Cases,
+   count(distinct samp) AS Samples,
+    count(distinct cf) AS `Case Files`,
+    count(distinct sf) AS `Study Files`</t>
+  </si>
+  <si>
+    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
+MATCH (c)&lt;--(diag:diagnosis)
+OPTIONAL MATCH (co:cohort)&lt;-[*]-(c)
+MATCH (samp:sample)--&gt;(c)
+WHERE  samp.specific_sample_pathology in ['Astrocytoma']
+WITH DISTINCT c, s, demo, diag, co, demo.patient_age_at_enrollment AS age, demo.weight as weight
+RETURN  coalesce(c.case_id, '') AS `Case ID` ,
+        coalesce(s.clinical_study_designation, '') AS `Study Code` ,
+        coalesce(s.clinical_study_type, '') AS  `Study Type`,
+        coalesce(demo.breed, '') AS Breed ,
+        coalesce(diag.disease_term, '') AS Diagnosis ,
+        coalesce(diag.stage_of_disease, '') AS `Stage of Disease` ,
+  coalesce(CASE age % 1 WHEN 0 THEN apoc.convert.toInteger(age) ELSE age END, '') AS Age,
+       coalesce(demo.sex, '') AS Sex,
+       coalesce(demo.neutered_indicator, '') AS `Neutered Status`,
+coalesce(CASE weight % 1 WHEN 0 THEN apoc.convert.toInteger(weight) ELSE weight END, '') AS `Weight (kg)`,
+       coalesce(diag.best_response, '') AS `Response to Treatment`,
+       coalesce(co.cohort_description, '') AS `Cohort`
+order by c.case_id asc
+limit 100</t>
   </si>
   <si>
     <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (samp:sample)--&gt;(c)&lt;--(diag:diagnosis) 
- WHERE samp.specific_sample_pathology IN ["Astrocytoma"]  
+WHERE  samp.specific_sample_pathology IN ['Astrocytoma']
 WITH DISTINCT samp AS samp, c, demo, diag
 RETURN  coalesce(samp.sample_id, '') AS `Sample ID`, 
         coalesce(c.case_id, '') AS `Case ID`, 
-        coalesce(demo.breed,'') AS Breed , 
-        coalesce(diag.disease_term,'') AS Diagnosis , 
+        coalesce(demo.breed,'') AS Breed,
+        coalesce(diag.disease_term,'') AS Diagnosis, 
         coalesce(samp.sample_site, '') AS `Sample Site`,
         coalesce(samp.summarized_sample_type, '') AS `Sample Type`,
         coalesce(samp.specific_sample_pathology, '') AS `Pathology/Morphology`,
@@ -93,50 +159,51 @@
         coalesce(samp.sample_chronology, '') AS `Sample Chronology`,
         coalesce(samp.percentage_tumor, '') AS `Percentage Tumor`,
         coalesce(samp.necropsy_sample, '') AS `Necropsy Sample`,
-        coalesce(samp.sample_preservation, '') AS `Sample Preservation`</t>
+        coalesce(samp.sample_preservation, '') AS `Sample Preservation`
+order by samp.sample_id asc
+limit 200</t>
   </si>
   <si>
     <t>MATCH (f:file)--&gt;(parent)
 WITH DISTINCT f, parent
 MATCH (f)-[*]-&gt;(c:case)&lt;--(demo:demographic)
- MATCH (s:study)&lt;-[*]-(c)&lt;--(diag:diagnosis)
- MATCH (samp:sample)--&gt;(c) 
- WHERE samp.specific_sample_pathology IN ["Astrocytoma"]  
-WITH DISTINCT f, parent, c, demo, diag, s
-RETURN coalesce(f.file_name, '') AS `File Name`, 
+MATCH (s:study)&lt;-[*]-(c)&lt;--(diag:diagnosis)
+MATCH (f)--&gt;(samp:sample)
+WHERE samp.specific_sample_pathology IN ['Astrocytoma']
+ MATCH (f)-[*]-&gt;(samp:sample)
+WITH
+        DISTINCT f, parent, c, demo, diag, s, samp,
+        ['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units,
+        toInteger(floor(log(f.file_size)/log(1024))) as i,
+        2 as precision
+WITH
+        f, parent, c, demo, diag, s, samp,
+        f.file_size /(1024^i) AS value,
+        10^precision AS factor,
+        units[i] as unit
+WITH
+        f, parent, c, demo, diag, s, samp, unit,
+        round(factor * value)/factor AS size
+RETURN
+        coalesce(f.file_name, '') AS `File Name`,
+        coalesce(f.file_format, '') AS `Format`,
+        coalesce(f.file_type, '') AS `File Type`,
+        CASE size % 1 WHEN 0 THEN apoc.convert.toInteger(size)+' ' +unit ELSE size+' ' +unit END AS Size,
         coalesce(labels(parent)[0], '') AS `Association`,
         coalesce(f.file_description, '') AS `Description`,
-        coalesce(f.file_format, '') AS `Format`,
-        coalesce(f.file_size, '') AS `Size`,
-        coalesce(c.case_id, '') AS `Case ID`, 
-        coalesce(diag.disease_term,'') AS Diagnosis , 
-        coalesce(s.clinical_study_designation,'') AS `Study Code`</t>
-  </si>
-  <si>
-    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
-MATCH (c)&lt;--(diag:diagnosis)
-MATCH (samp:sample)--&gt;(c) 
- WHERE samp.specific_sample_pathology IN ["Astrocytoma"]  
-OPTIONAL MATCH (co:cohort)&lt;-[*]-(c)
-  WITH DISTINCT c, s, demo, diag, co
-RETURN  coalesce(c.case_id, '') AS `Case ID` ,
-        coalesce(s.clinical_study_designation, '') AS `Study Code` ,
-        coalesce(s.clinical_study_type, '') AS  `Study Type`,
-        coalesce(demo.breed, '') AS Breed ,
-        coalesce(diag.disease_term, '') AS Diagnosis ,
-        coalesce(diag.stage_of_disease, '') AS `Stage of Disease` ,
-        coalesce(demo.patient_age_at_enrollment, '') AS Age ,
-        coalesce(demo.sex, '') AS Sex ,
-        coalesce(demo.neutered_indicator, '') AS `Neutered Status`,
-        coalesce(demo.weight, '') AS `Weight (kg)`,
-        coalesce(diag.best_response, '') AS `Response to Treatment`</t>
+        coalesce(samp.sample_id, '') AS `Sample ID`,
+        coalesce(c.case_id, '') AS `Case ID`,
+        coalesce(demo.breed,'') AS Breed ,
+        coalesce(diag.disease_term,'') AS Diagnosis
+        order by f.file_name asc
+        limit 100</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -153,6 +220,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -179,9 +253,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -499,22 +579,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="87.6640625" customWidth="1"/>
-    <col min="3" max="3" width="75.77734375" customWidth="1"/>
-    <col min="4" max="4" width="70.21875" customWidth="1"/>
-    <col min="5" max="5" width="28.5546875" customWidth="1"/>
+    <col min="1" max="1" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="87.6328125" customWidth="1"/>
+    <col min="3" max="3" width="75.81640625" customWidth="1"/>
+    <col min="4" max="4" width="70.1796875" customWidth="1"/>
+    <col min="5" max="5" width="28.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -531,15 +611,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="244.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="304.5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
@@ -548,15 +628,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="244.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>10</v>
+      <c r="B3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
@@ -565,20 +645,37 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="244.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="409.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="D4" t="s">
         <v>8</v>
       </c>
       <c r="E4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="409.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>